<commit_message>
renamed resetPopulation to setPopulation; added sections to interactive_use_tutorial
</commit_message>
<xml_diff>
--- a/inst/testdata/qcPed.xlsx
+++ b/inst/testdata/qcPed.xlsx
@@ -1,29 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/msharp/Documents/Development/R/r_workspace/library/nprcmanager/inst/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E05D7DB5-50A8-6D41-A049-3395B623A281}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DE09ABAC-8CF4-9F46-88FA-B05339E5B598}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3180" yWindow="2060" windowWidth="27640" windowHeight="16940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440"/>
   </bookViews>
   <sheets>
     <sheet name="qcPed" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -909,10 +901,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
-  </numFmts>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1392,7 +1381,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1747,17 +1736,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H281"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="6" max="7" width="10.83203125" style="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -1775,10 +1759,10 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
       <c r="H1" t="s">
@@ -1801,7 +1785,7 @@
       <c r="E2">
         <v>0</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" t="s">
         <v>9</v>
       </c>
       <c r="G2" s="1">
@@ -1986,7 +1970,7 @@
       <c r="F9" s="1">
         <v>35140</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="G9" t="s">
         <v>9</v>
       </c>
       <c r="H9">
@@ -2503,7 +2487,7 @@
       <c r="E29">
         <v>0</v>
       </c>
-      <c r="F29" s="1" t="s">
+      <c r="F29" t="s">
         <v>9</v>
       </c>
       <c r="G29" s="1">
@@ -2529,7 +2513,7 @@
       <c r="E30">
         <v>0</v>
       </c>
-      <c r="F30" s="1" t="s">
+      <c r="F30" t="s">
         <v>9</v>
       </c>
       <c r="G30" s="1">
@@ -2763,7 +2747,7 @@
       <c r="E39">
         <v>0</v>
       </c>
-      <c r="F39" s="1" t="s">
+      <c r="F39" t="s">
         <v>9</v>
       </c>
       <c r="G39" s="1">
@@ -3832,7 +3816,7 @@
       <c r="F80" s="1">
         <v>38520</v>
       </c>
-      <c r="G80" s="1" t="s">
+      <c r="G80" t="s">
         <v>9</v>
       </c>
       <c r="H80">
@@ -3907,10 +3891,10 @@
       <c r="E83">
         <v>0</v>
       </c>
-      <c r="F83" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G83" s="1" t="s">
+      <c r="F83" t="s">
+        <v>9</v>
+      </c>
+      <c r="G83" t="s">
         <v>9</v>
       </c>
       <c r="H83" t="s">
@@ -3933,10 +3917,10 @@
       <c r="E84">
         <v>0</v>
       </c>
-      <c r="F84" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G84" s="1" t="s">
+      <c r="F84" t="s">
+        <v>9</v>
+      </c>
+      <c r="G84" t="s">
         <v>9</v>
       </c>
       <c r="H84" t="s">
@@ -3959,10 +3943,10 @@
       <c r="E85">
         <v>0</v>
       </c>
-      <c r="F85" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G85" s="1" t="s">
+      <c r="F85" t="s">
+        <v>9</v>
+      </c>
+      <c r="G85" t="s">
         <v>9</v>
       </c>
       <c r="H85" t="s">
@@ -3985,10 +3969,10 @@
       <c r="E86">
         <v>0</v>
       </c>
-      <c r="F86" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G86" s="1" t="s">
+      <c r="F86" t="s">
+        <v>9</v>
+      </c>
+      <c r="G86" t="s">
         <v>9</v>
       </c>
       <c r="H86" t="s">
@@ -4011,10 +3995,10 @@
       <c r="E87">
         <v>0</v>
       </c>
-      <c r="F87" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G87" s="1" t="s">
+      <c r="F87" t="s">
+        <v>9</v>
+      </c>
+      <c r="G87" t="s">
         <v>9</v>
       </c>
       <c r="H87" t="s">
@@ -4037,10 +4021,10 @@
       <c r="E88">
         <v>0</v>
       </c>
-      <c r="F88" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G88" s="1" t="s">
+      <c r="F88" t="s">
+        <v>9</v>
+      </c>
+      <c r="G88" t="s">
         <v>9</v>
       </c>
       <c r="H88" t="s">
@@ -4063,10 +4047,10 @@
       <c r="E89">
         <v>0</v>
       </c>
-      <c r="F89" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G89" s="1" t="s">
+      <c r="F89" t="s">
+        <v>9</v>
+      </c>
+      <c r="G89" t="s">
         <v>9</v>
       </c>
       <c r="H89" t="s">
@@ -4089,10 +4073,10 @@
       <c r="E90">
         <v>0</v>
       </c>
-      <c r="F90" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G90" s="1" t="s">
+      <c r="F90" t="s">
+        <v>9</v>
+      </c>
+      <c r="G90" t="s">
         <v>9</v>
       </c>
       <c r="H90" t="s">
@@ -4115,10 +4099,10 @@
       <c r="E91">
         <v>0</v>
       </c>
-      <c r="F91" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G91" s="1" t="s">
+      <c r="F91" t="s">
+        <v>9</v>
+      </c>
+      <c r="G91" t="s">
         <v>9</v>
       </c>
       <c r="H91" t="s">
@@ -4141,10 +4125,10 @@
       <c r="E92">
         <v>0</v>
       </c>
-      <c r="F92" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G92" s="1" t="s">
+      <c r="F92" t="s">
+        <v>9</v>
+      </c>
+      <c r="G92" t="s">
         <v>9</v>
       </c>
       <c r="H92" t="s">
@@ -4167,10 +4151,10 @@
       <c r="E93">
         <v>0</v>
       </c>
-      <c r="F93" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G93" s="1" t="s">
+      <c r="F93" t="s">
+        <v>9</v>
+      </c>
+      <c r="G93" t="s">
         <v>9</v>
       </c>
       <c r="H93" t="s">
@@ -4193,10 +4177,10 @@
       <c r="E94">
         <v>0</v>
       </c>
-      <c r="F94" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G94" s="1" t="s">
+      <c r="F94" t="s">
+        <v>9</v>
+      </c>
+      <c r="G94" t="s">
         <v>9</v>
       </c>
       <c r="H94" t="s">
@@ -4219,10 +4203,10 @@
       <c r="E95">
         <v>0</v>
       </c>
-      <c r="F95" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G95" s="1" t="s">
+      <c r="F95" t="s">
+        <v>9</v>
+      </c>
+      <c r="G95" t="s">
         <v>9</v>
       </c>
       <c r="H95" t="s">
@@ -4245,10 +4229,10 @@
       <c r="E96">
         <v>0</v>
       </c>
-      <c r="F96" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G96" s="1" t="s">
+      <c r="F96" t="s">
+        <v>9</v>
+      </c>
+      <c r="G96" t="s">
         <v>9</v>
       </c>
       <c r="H96" t="s">
@@ -4271,10 +4255,10 @@
       <c r="E97">
         <v>0</v>
       </c>
-      <c r="F97" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G97" s="1" t="s">
+      <c r="F97" t="s">
+        <v>9</v>
+      </c>
+      <c r="G97" t="s">
         <v>9</v>
       </c>
       <c r="H97" t="s">
@@ -4297,10 +4281,10 @@
       <c r="E98">
         <v>0</v>
       </c>
-      <c r="F98" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G98" s="1" t="s">
+      <c r="F98" t="s">
+        <v>9</v>
+      </c>
+      <c r="G98" t="s">
         <v>9</v>
       </c>
       <c r="H98" t="s">
@@ -4323,10 +4307,10 @@
       <c r="E99">
         <v>0</v>
       </c>
-      <c r="F99" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G99" s="1" t="s">
+      <c r="F99" t="s">
+        <v>9</v>
+      </c>
+      <c r="G99" t="s">
         <v>9</v>
       </c>
       <c r="H99" t="s">
@@ -4349,10 +4333,10 @@
       <c r="E100">
         <v>0</v>
       </c>
-      <c r="F100" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G100" s="1" t="s">
+      <c r="F100" t="s">
+        <v>9</v>
+      </c>
+      <c r="G100" t="s">
         <v>9</v>
       </c>
       <c r="H100" t="s">
@@ -4375,10 +4359,10 @@
       <c r="E101">
         <v>0</v>
       </c>
-      <c r="F101" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G101" s="1" t="s">
+      <c r="F101" t="s">
+        <v>9</v>
+      </c>
+      <c r="G101" t="s">
         <v>9</v>
       </c>
       <c r="H101" t="s">
@@ -4401,10 +4385,10 @@
       <c r="E102">
         <v>0</v>
       </c>
-      <c r="F102" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G102" s="1" t="s">
+      <c r="F102" t="s">
+        <v>9</v>
+      </c>
+      <c r="G102" t="s">
         <v>9</v>
       </c>
       <c r="H102" t="s">
@@ -4427,10 +4411,10 @@
       <c r="E103">
         <v>0</v>
       </c>
-      <c r="F103" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G103" s="1" t="s">
+      <c r="F103" t="s">
+        <v>9</v>
+      </c>
+      <c r="G103" t="s">
         <v>9</v>
       </c>
       <c r="H103" t="s">
@@ -4453,10 +4437,10 @@
       <c r="E104">
         <v>0</v>
       </c>
-      <c r="F104" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G104" s="1" t="s">
+      <c r="F104" t="s">
+        <v>9</v>
+      </c>
+      <c r="G104" t="s">
         <v>9</v>
       </c>
       <c r="H104" t="s">
@@ -4479,10 +4463,10 @@
       <c r="E105">
         <v>0</v>
       </c>
-      <c r="F105" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G105" s="1" t="s">
+      <c r="F105" t="s">
+        <v>9</v>
+      </c>
+      <c r="G105" t="s">
         <v>9</v>
       </c>
       <c r="H105" t="s">
@@ -4505,10 +4489,10 @@
       <c r="E106">
         <v>0</v>
       </c>
-      <c r="F106" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G106" s="1" t="s">
+      <c r="F106" t="s">
+        <v>9</v>
+      </c>
+      <c r="G106" t="s">
         <v>9</v>
       </c>
       <c r="H106" t="s">
@@ -4531,10 +4515,10 @@
       <c r="E107">
         <v>0</v>
       </c>
-      <c r="F107" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G107" s="1" t="s">
+      <c r="F107" t="s">
+        <v>9</v>
+      </c>
+      <c r="G107" t="s">
         <v>9</v>
       </c>
       <c r="H107" t="s">
@@ -4557,10 +4541,10 @@
       <c r="E108">
         <v>0</v>
       </c>
-      <c r="F108" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G108" s="1" t="s">
+      <c r="F108" t="s">
+        <v>9</v>
+      </c>
+      <c r="G108" t="s">
         <v>9</v>
       </c>
       <c r="H108" t="s">
@@ -4583,10 +4567,10 @@
       <c r="E109">
         <v>0</v>
       </c>
-      <c r="F109" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G109" s="1" t="s">
+      <c r="F109" t="s">
+        <v>9</v>
+      </c>
+      <c r="G109" t="s">
         <v>9</v>
       </c>
       <c r="H109" t="s">
@@ -4609,10 +4593,10 @@
       <c r="E110">
         <v>0</v>
       </c>
-      <c r="F110" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G110" s="1" t="s">
+      <c r="F110" t="s">
+        <v>9</v>
+      </c>
+      <c r="G110" t="s">
         <v>9</v>
       </c>
       <c r="H110" t="s">
@@ -4635,10 +4619,10 @@
       <c r="E111">
         <v>0</v>
       </c>
-      <c r="F111" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G111" s="1" t="s">
+      <c r="F111" t="s">
+        <v>9</v>
+      </c>
+      <c r="G111" t="s">
         <v>9</v>
       </c>
       <c r="H111" t="s">
@@ -4661,10 +4645,10 @@
       <c r="E112">
         <v>0</v>
       </c>
-      <c r="F112" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G112" s="1" t="s">
+      <c r="F112" t="s">
+        <v>9</v>
+      </c>
+      <c r="G112" t="s">
         <v>9</v>
       </c>
       <c r="H112" t="s">
@@ -4687,10 +4671,10 @@
       <c r="E113">
         <v>0</v>
       </c>
-      <c r="F113" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G113" s="1" t="s">
+      <c r="F113" t="s">
+        <v>9</v>
+      </c>
+      <c r="G113" t="s">
         <v>9</v>
       </c>
       <c r="H113" t="s">
@@ -4713,10 +4697,10 @@
       <c r="E114">
         <v>0</v>
       </c>
-      <c r="F114" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G114" s="1" t="s">
+      <c r="F114" t="s">
+        <v>9</v>
+      </c>
+      <c r="G114" t="s">
         <v>9</v>
       </c>
       <c r="H114" t="s">
@@ -4739,10 +4723,10 @@
       <c r="E115">
         <v>0</v>
       </c>
-      <c r="F115" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G115" s="1" t="s">
+      <c r="F115" t="s">
+        <v>9</v>
+      </c>
+      <c r="G115" t="s">
         <v>9</v>
       </c>
       <c r="H115" t="s">
@@ -4765,10 +4749,10 @@
       <c r="E116">
         <v>0</v>
       </c>
-      <c r="F116" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G116" s="1" t="s">
+      <c r="F116" t="s">
+        <v>9</v>
+      </c>
+      <c r="G116" t="s">
         <v>9</v>
       </c>
       <c r="H116" t="s">
@@ -4791,10 +4775,10 @@
       <c r="E117">
         <v>0</v>
       </c>
-      <c r="F117" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G117" s="1" t="s">
+      <c r="F117" t="s">
+        <v>9</v>
+      </c>
+      <c r="G117" t="s">
         <v>9</v>
       </c>
       <c r="H117" t="s">
@@ -4817,10 +4801,10 @@
       <c r="E118">
         <v>0</v>
       </c>
-      <c r="F118" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G118" s="1" t="s">
+      <c r="F118" t="s">
+        <v>9</v>
+      </c>
+      <c r="G118" t="s">
         <v>9</v>
       </c>
       <c r="H118" t="s">
@@ -4843,10 +4827,10 @@
       <c r="E119">
         <v>0</v>
       </c>
-      <c r="F119" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G119" s="1" t="s">
+      <c r="F119" t="s">
+        <v>9</v>
+      </c>
+      <c r="G119" t="s">
         <v>9</v>
       </c>
       <c r="H119" t="s">
@@ -4869,10 +4853,10 @@
       <c r="E120">
         <v>0</v>
       </c>
-      <c r="F120" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G120" s="1" t="s">
+      <c r="F120" t="s">
+        <v>9</v>
+      </c>
+      <c r="G120" t="s">
         <v>9</v>
       </c>
       <c r="H120" t="s">
@@ -4895,10 +4879,10 @@
       <c r="E121">
         <v>0</v>
       </c>
-      <c r="F121" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G121" s="1" t="s">
+      <c r="F121" t="s">
+        <v>9</v>
+      </c>
+      <c r="G121" t="s">
         <v>9</v>
       </c>
       <c r="H121" t="s">
@@ -4921,10 +4905,10 @@
       <c r="E122">
         <v>0</v>
       </c>
-      <c r="F122" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G122" s="1" t="s">
+      <c r="F122" t="s">
+        <v>9</v>
+      </c>
+      <c r="G122" t="s">
         <v>9</v>
       </c>
       <c r="H122" t="s">
@@ -4947,10 +4931,10 @@
       <c r="E123">
         <v>0</v>
       </c>
-      <c r="F123" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G123" s="1" t="s">
+      <c r="F123" t="s">
+        <v>9</v>
+      </c>
+      <c r="G123" t="s">
         <v>9</v>
       </c>
       <c r="H123" t="s">
@@ -4973,10 +4957,10 @@
       <c r="E124">
         <v>0</v>
       </c>
-      <c r="F124" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G124" s="1" t="s">
+      <c r="F124" t="s">
+        <v>9</v>
+      </c>
+      <c r="G124" t="s">
         <v>9</v>
       </c>
       <c r="H124" t="s">
@@ -4999,10 +4983,10 @@
       <c r="E125">
         <v>0</v>
       </c>
-      <c r="F125" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G125" s="1" t="s">
+      <c r="F125" t="s">
+        <v>9</v>
+      </c>
+      <c r="G125" t="s">
         <v>9</v>
       </c>
       <c r="H125" t="s">
@@ -5990,7 +5974,7 @@
       <c r="F163" s="1">
         <v>38333</v>
       </c>
-      <c r="G163" s="1" t="s">
+      <c r="G163" t="s">
         <v>9</v>
       </c>
       <c r="H163">
@@ -6874,7 +6858,7 @@
       <c r="F197" s="1">
         <v>36114</v>
       </c>
-      <c r="G197" s="1" t="s">
+      <c r="G197" t="s">
         <v>9</v>
       </c>
       <c r="H197">
@@ -7004,7 +6988,7 @@
       <c r="F202" s="1">
         <v>38046</v>
       </c>
-      <c r="G202" s="1" t="s">
+      <c r="G202" t="s">
         <v>9</v>
       </c>
       <c r="H202">
@@ -7134,7 +7118,7 @@
       <c r="F207" s="1">
         <v>38438</v>
       </c>
-      <c r="G207" s="1" t="s">
+      <c r="G207" t="s">
         <v>9</v>
       </c>
       <c r="H207">
@@ -7160,7 +7144,7 @@
       <c r="F208" s="1">
         <v>38395</v>
       </c>
-      <c r="G208" s="1" t="s">
+      <c r="G208" t="s">
         <v>9</v>
       </c>
       <c r="H208">
@@ -7186,7 +7170,7 @@
       <c r="F209" s="1">
         <v>42421</v>
       </c>
-      <c r="G209" s="1" t="s">
+      <c r="G209" t="s">
         <v>9</v>
       </c>
       <c r="H209">
@@ -7732,7 +7716,7 @@
       <c r="F230" s="1">
         <v>36141</v>
       </c>
-      <c r="G230" s="1" t="s">
+      <c r="G230" t="s">
         <v>9</v>
       </c>
       <c r="H230">
@@ -7862,7 +7846,7 @@
       <c r="F235" s="1">
         <v>36396</v>
       </c>
-      <c r="G235" s="1" t="s">
+      <c r="G235" t="s">
         <v>9</v>
       </c>
       <c r="H235">
@@ -7888,7 +7872,7 @@
       <c r="F236" s="1">
         <v>36473</v>
       </c>
-      <c r="G236" s="1" t="s">
+      <c r="G236" t="s">
         <v>9</v>
       </c>
       <c r="H236">
@@ -7966,7 +7950,7 @@
       <c r="F239" s="1">
         <v>36916</v>
       </c>
-      <c r="G239" s="1" t="s">
+      <c r="G239" t="s">
         <v>9</v>
       </c>
       <c r="H239">
@@ -8070,7 +8054,7 @@
       <c r="F243" s="1">
         <v>38268</v>
       </c>
-      <c r="G243" s="1" t="s">
+      <c r="G243" t="s">
         <v>9</v>
       </c>
       <c r="H243">
@@ -8148,7 +8132,7 @@
       <c r="F246" s="1">
         <v>38696</v>
       </c>
-      <c r="G246" s="1" t="s">
+      <c r="G246" t="s">
         <v>9</v>
       </c>
       <c r="H246">
@@ -8174,7 +8158,7 @@
       <c r="F247" s="1">
         <v>38744</v>
       </c>
-      <c r="G247" s="1" t="s">
+      <c r="G247" t="s">
         <v>9</v>
       </c>
       <c r="H247">
@@ -8200,7 +8184,7 @@
       <c r="F248" s="1">
         <v>38831</v>
       </c>
-      <c r="G248" s="1" t="s">
+      <c r="G248" t="s">
         <v>9</v>
       </c>
       <c r="H248">
@@ -8226,7 +8210,7 @@
       <c r="F249" s="1">
         <v>38860</v>
       </c>
-      <c r="G249" s="1" t="s">
+      <c r="G249" t="s">
         <v>9</v>
       </c>
       <c r="H249">
@@ -8252,7 +8236,7 @@
       <c r="F250" s="1">
         <v>38922</v>
       </c>
-      <c r="G250" s="1" t="s">
+      <c r="G250" t="s">
         <v>9</v>
       </c>
       <c r="H250">
@@ -8278,7 +8262,7 @@
       <c r="F251" s="1">
         <v>39165</v>
       </c>
-      <c r="G251" s="1" t="s">
+      <c r="G251" t="s">
         <v>9</v>
       </c>
       <c r="H251">
@@ -8304,7 +8288,7 @@
       <c r="F252" s="1">
         <v>41443</v>
       </c>
-      <c r="G252" s="1" t="s">
+      <c r="G252" t="s">
         <v>9</v>
       </c>
       <c r="H252">
@@ -8330,7 +8314,7 @@
       <c r="F253" s="1">
         <v>42013</v>
       </c>
-      <c r="G253" s="1" t="s">
+      <c r="G253" t="s">
         <v>9</v>
       </c>
       <c r="H253">
@@ -8356,7 +8340,7 @@
       <c r="F254" s="1">
         <v>42034</v>
       </c>
-      <c r="G254" s="1" t="s">
+      <c r="G254" t="s">
         <v>9</v>
       </c>
       <c r="H254">
@@ -8382,7 +8366,7 @@
       <c r="F255" s="1">
         <v>42042</v>
       </c>
-      <c r="G255" s="1" t="s">
+      <c r="G255" t="s">
         <v>9</v>
       </c>
       <c r="H255">
@@ -8434,7 +8418,7 @@
       <c r="F257" s="1">
         <v>42259</v>
       </c>
-      <c r="G257" s="1" t="s">
+      <c r="G257" t="s">
         <v>9</v>
       </c>
       <c r="H257">
@@ -8512,7 +8496,7 @@
       <c r="F260" s="1">
         <v>38712</v>
       </c>
-      <c r="G260" s="1" t="s">
+      <c r="G260" t="s">
         <v>9</v>
       </c>
       <c r="H260">
@@ -8538,7 +8522,7 @@
       <c r="F261" s="1">
         <v>39376</v>
       </c>
-      <c r="G261" s="1" t="s">
+      <c r="G261" t="s">
         <v>9</v>
       </c>
       <c r="H261">
@@ -8564,7 +8548,7 @@
       <c r="F262" s="1">
         <v>41065</v>
       </c>
-      <c r="G262" s="1" t="s">
+      <c r="G262" t="s">
         <v>9</v>
       </c>
       <c r="H262">
@@ -8590,7 +8574,7 @@
       <c r="F263" s="1">
         <v>41301</v>
       </c>
-      <c r="G263" s="1" t="s">
+      <c r="G263" t="s">
         <v>9</v>
       </c>
       <c r="H263">
@@ -8616,7 +8600,7 @@
       <c r="F264" s="1">
         <v>41350</v>
       </c>
-      <c r="G264" s="1" t="s">
+      <c r="G264" t="s">
         <v>9</v>
       </c>
       <c r="H264">
@@ -8642,7 +8626,7 @@
       <c r="F265" s="1">
         <v>41415</v>
       </c>
-      <c r="G265" s="1" t="s">
+      <c r="G265" t="s">
         <v>9</v>
       </c>
       <c r="H265">
@@ -8668,7 +8652,7 @@
       <c r="F266" s="1">
         <v>41427</v>
       </c>
-      <c r="G266" s="1" t="s">
+      <c r="G266" t="s">
         <v>9</v>
       </c>
       <c r="H266">
@@ -8694,7 +8678,7 @@
       <c r="F267" s="1">
         <v>41457</v>
       </c>
-      <c r="G267" s="1" t="s">
+      <c r="G267" t="s">
         <v>9</v>
       </c>
       <c r="H267">
@@ -8720,7 +8704,7 @@
       <c r="F268" s="1">
         <v>41490</v>
       </c>
-      <c r="G268" s="1" t="s">
+      <c r="G268" t="s">
         <v>9</v>
       </c>
       <c r="H268">
@@ -8746,7 +8730,7 @@
       <c r="F269" s="1">
         <v>41729</v>
       </c>
-      <c r="G269" s="1" t="s">
+      <c r="G269" t="s">
         <v>9</v>
       </c>
       <c r="H269">
@@ -8772,7 +8756,7 @@
       <c r="F270" s="1">
         <v>41935</v>
       </c>
-      <c r="G270" s="1" t="s">
+      <c r="G270" t="s">
         <v>9</v>
       </c>
       <c r="H270">
@@ -8798,7 +8782,7 @@
       <c r="F271" s="1">
         <v>42018</v>
       </c>
-      <c r="G271" s="1" t="s">
+      <c r="G271" t="s">
         <v>9</v>
       </c>
       <c r="H271">
@@ -8824,7 +8808,7 @@
       <c r="F272" s="1">
         <v>42043</v>
       </c>
-      <c r="G272" s="1" t="s">
+      <c r="G272" t="s">
         <v>9</v>
       </c>
       <c r="H272">
@@ -8850,7 +8834,7 @@
       <c r="F273" s="1">
         <v>42058</v>
       </c>
-      <c r="G273" s="1" t="s">
+      <c r="G273" t="s">
         <v>9</v>
       </c>
       <c r="H273">
@@ -8876,7 +8860,7 @@
       <c r="F274" s="1">
         <v>42026</v>
       </c>
-      <c r="G274" s="1" t="s">
+      <c r="G274" t="s">
         <v>9</v>
       </c>
       <c r="H274">
@@ -8902,7 +8886,7 @@
       <c r="F275" s="1">
         <v>42084</v>
       </c>
-      <c r="G275" s="1" t="s">
+      <c r="G275" t="s">
         <v>9</v>
       </c>
       <c r="H275">
@@ -8928,7 +8912,7 @@
       <c r="F276" s="1">
         <v>42151</v>
       </c>
-      <c r="G276" s="1" t="s">
+      <c r="G276" t="s">
         <v>9</v>
       </c>
       <c r="H276">
@@ -8954,7 +8938,7 @@
       <c r="F277" s="1">
         <v>42242</v>
       </c>
-      <c r="G277" s="1" t="s">
+      <c r="G277" t="s">
         <v>9</v>
       </c>
       <c r="H277">
@@ -8980,7 +8964,7 @@
       <c r="F278" s="1">
         <v>42509</v>
       </c>
-      <c r="G278" s="1" t="s">
+      <c r="G278" t="s">
         <v>9</v>
       </c>
       <c r="H278">
@@ -9006,7 +8990,7 @@
       <c r="F279" s="1">
         <v>41416</v>
       </c>
-      <c r="G279" s="1" t="s">
+      <c r="G279" t="s">
         <v>9</v>
       </c>
       <c r="H279">
@@ -9032,7 +9016,7 @@
       <c r="F280" s="1">
         <v>41679</v>
       </c>
-      <c r="G280" s="1" t="s">
+      <c r="G280" t="s">
         <v>9</v>
       </c>
       <c r="H280">
@@ -9058,7 +9042,7 @@
       <c r="F281" s="1">
         <v>42301</v>
       </c>
-      <c r="G281" s="1" t="s">
+      <c r="G281" t="s">
         <v>9</v>
       </c>
       <c r="H281">

</xml_diff>